<commit_message>
Fixed freezing by creating a HTMLSession object for each url
</commit_message>
<xml_diff>
--- a/DetectInputField/webpages_inputdata.xlsx
+++ b/DetectInputField/webpages_inputdata.xlsx
@@ -4,18 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
     <sheet name="Keywords" sheetId="2" r:id="rId2"/>
+    <sheet name="Output" sheetId="3" r:id="rId3"/>
+    <sheet name="Errors" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="50">
   <si>
     <t>URL</t>
   </si>
@@ -26,19 +28,91 @@
     <t>theraflu.com/products/sinus-and-pain-product</t>
   </si>
   <si>
-    <t>tums.com/antacid-products/chewy-bites-gas-relief</t>
-  </si>
-  <si>
     <t>terveys.gsk.fi/fi-fi/_adverse-effect-reportage</t>
   </si>
   <si>
-    <t>sensodyne.co.uk</t>
-  </si>
-  <si>
     <t>https://www.caltrate.co.za/caltrate-plus-chewables</t>
   </si>
   <si>
-    <t>10ubun.lt</t>
+    <t>100budu.lt</t>
+  </si>
+  <si>
+    <t>parodontax.com.ar</t>
+  </si>
+  <si>
+    <t>parodontax.at</t>
+  </si>
+  <si>
+    <t>parodontax.be</t>
+  </si>
+  <si>
+    <t>36bushels.com</t>
+  </si>
+  <si>
+    <t>5euro-sparen.de</t>
+  </si>
+  <si>
+    <t>7keystohelp.dk</t>
+  </si>
+  <si>
+    <t>7keystohelp.no</t>
+  </si>
+  <si>
+    <t>7keystohelp.se</t>
+  </si>
+  <si>
+    <t>boostcamp.com</t>
+  </si>
+  <si>
+    <t>abreva.com</t>
+  </si>
+  <si>
+    <t>acneaidth.com</t>
+  </si>
+  <si>
+    <t>activir.fr</t>
+  </si>
+  <si>
+    <t>activir.jp</t>
+  </si>
+  <si>
+    <t>activp.fr</t>
+  </si>
+  <si>
+    <t>advil.ca</t>
+  </si>
+  <si>
+    <t>advil.ca/fr</t>
+  </si>
+  <si>
+    <t>advil.co.nz</t>
+  </si>
+  <si>
+    <t>advil.com</t>
+  </si>
+  <si>
+    <t>advil.com.br</t>
+  </si>
+  <si>
+    <t>advil.com.co</t>
+  </si>
+  <si>
+    <t>advil.com.mx</t>
+  </si>
+  <si>
+    <t>advil.com/es</t>
+  </si>
+  <si>
+    <t>advil.fr</t>
+  </si>
+  <si>
+    <t>advil.hu</t>
+  </si>
+  <si>
+    <t>abreva.ca</t>
+  </si>
+  <si>
+    <t>abreva.ca/fr_CA</t>
   </si>
   <si>
     <t>Keywords</t>
@@ -60,13 +134,46 @@
   </si>
   <si>
     <t>feedback</t>
+  </si>
+  <si>
+    <t>Can Input</t>
+  </si>
+  <si>
+    <t>Keyword Found</t>
+  </si>
+  <si>
+    <t>Navigation Timeout Exceeded: 10000 ms exceeded.</t>
+  </si>
+  <si>
+    <t>https://100budu.lt</t>
+  </si>
+  <si>
+    <t>HTTPSConnectionPool(host='100budu.lt', port=443): Max retries exceeded with url: / (Caused by NewConnectionError('&lt;urllib3.connection.HTTPSConnection object at 0x000001D5204CDAC0&gt;: Failed to establish a new connection: [Errno 11001] getaddrinfo failed'))</t>
+  </si>
+  <si>
+    <t>https://5euro-sparen.de</t>
+  </si>
+  <si>
+    <t>HTTPSConnectionPool(host='5euro-sparen.de', port=443): Max retries exceeded with url: / (Caused by NewConnectionError('&lt;urllib3.connection.HTTPSConnection object at 0x000001D51F357490&gt;: Failed to establish a new connection: [Errno 11001] getaddrinfo failed'))</t>
+  </si>
+  <si>
+    <t>https://7keystohelp.no</t>
+  </si>
+  <si>
+    <t>HTTPSConnectionPool(host='7keystohelp.no', port=443): Max retries exceeded with url: / (Caused by NewConnectionError('&lt;urllib3.connection.HTTPSConnection object at 0x000001D51F400EB0&gt;: Failed to establish a new connection: [Errno 11001] getaddrinfo failed'))</t>
+  </si>
+  <si>
+    <t>https://acneaidth.com</t>
+  </si>
+  <si>
+    <t>HTTPSConnectionPool(host='acneaidth.com', port=443): Max retries exceeded with url: / (Caused by ConnectTimeoutError(&lt;urllib3.connection.HTTPSConnection object at 0x000001D51F416790&gt;, 'Connection to acneaidth.com timed out. (connect timeout=5)'))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +197,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +221,17 @@
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE8E8E8"/>
       </patternFill>
     </fill>
   </fills>
@@ -133,7 +263,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -142,6 +272,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -420,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,49 +566,167 @@
     <col min="1" max="1" width="63.7109375" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" display="https://www.freelancer.com/users/l.php?url=https:%2F%2Fwww.caltrate.co.za%2Fcaltrate-plus-chewables&amp;sig=3e605f1f86ea75dbd6d4d781ce5c34f524f8104938f156499c879961e5ca51de"/>
+    <hyperlink ref="A4" r:id="rId1" display="https://www.freelancer.com/users/l.php?url=https:%2F%2Fwww.caltrate.co.za%2Fcaltrate-plus-chewables&amp;sig=3e605f1f86ea75dbd6d4d781ce5c34f524f8104938f156499c879961e5ca51de"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -484,7 +737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -495,41 +748,907 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C84"/>
+  <sheetViews>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="20" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" t="b">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" t="b">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" t="b">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="b">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>1</v>
+      </c>
+      <c r="B22" t="b">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" t="b">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="b">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B31" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B42" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>15</v>
+      </c>
+      <c r="B44" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="b">
+        <v>1</v>
+      </c>
+      <c r="C45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" t="b">
+        <v>1</v>
+      </c>
+      <c r="C47" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>24</v>
+      </c>
+      <c r="B52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>25</v>
+      </c>
+      <c r="B53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54" t="b">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>29</v>
+      </c>
+      <c r="B57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>30</v>
+      </c>
+      <c r="B58" t="b">
+        <v>1</v>
+      </c>
+      <c r="C58" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B59" t="b">
+        <v>1</v>
+      </c>
+      <c r="C59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" t="b">
+        <v>1</v>
+      </c>
+      <c r="C60" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" t="b">
+        <v>1</v>
+      </c>
+      <c r="C61" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>7</v>
+      </c>
+      <c r="B64" t="b">
+        <v>1</v>
+      </c>
+      <c r="C64" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>11</v>
+      </c>
+      <c r="B66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>15</v>
+      </c>
+      <c r="B69" t="b">
+        <v>1</v>
+      </c>
+      <c r="C69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" t="b">
+        <v>1</v>
+      </c>
+      <c r="C70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" t="b">
+        <v>1</v>
+      </c>
+      <c r="C71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="b">
+        <v>1</v>
+      </c>
+      <c r="C72" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>21</v>
+      </c>
+      <c r="B74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>22</v>
+      </c>
+      <c r="B75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>23</v>
+      </c>
+      <c r="B76" t="b">
+        <v>1</v>
+      </c>
+      <c r="C76" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>25</v>
+      </c>
+      <c r="B78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>26</v>
+      </c>
+      <c r="B79" t="b">
+        <v>1</v>
+      </c>
+      <c r="C79" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>28</v>
+      </c>
+      <c r="B81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+      <c r="B82" t="b">
+        <v>1</v>
+      </c>
+      <c r="C82" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>30</v>
+      </c>
+      <c r="B83" t="b">
+        <v>1</v>
+      </c>
+      <c r="C83" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>31</v>
+      </c>
+      <c r="B84" t="b">
+        <v>1</v>
+      </c>
+      <c r="C84" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>